<commit_message>
more work on screen processing, works mostly but brittle
</commit_message>
<xml_diff>
--- a/think tank/fundamentals/v1.1/daily-price-demo.xlsx
+++ b/think tank/fundamentals/v1.1/daily-price-demo.xlsx
@@ -468,27 +468,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12.6400</t>
+          <t>137.5300</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12.6400</t>
+          <t>140.0000</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11.7600</t>
+          <t>137.2300</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12.4100</t>
+          <t>139.8700</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>128705</t>
+          <t>1851144</t>
         </is>
       </c>
     </row>
@@ -500,27 +500,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12.9100</t>
+          <t>135.9800</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>13.0900</t>
+          <t>137.9200</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12.3700</t>
+          <t>135.4300</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>12.5400</t>
+          <t>137.6300</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>66323</t>
+          <t>2425230</t>
         </is>
       </c>
     </row>
@@ -532,27 +532,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>13.0000</t>
+          <t>130.9300</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>13.1200</t>
+          <t>135.2700</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12.6500</t>
+          <t>130.7050</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>12.8700</t>
+          <t>135.1900</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>82560</t>
+          <t>1355167</t>
         </is>
       </c>
     </row>
@@ -564,27 +564,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13.2100</t>
+          <t>128.9700</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>13.4900</t>
+          <t>131.8250</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12.9200</t>
+          <t>128.6100</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>13.0700</t>
+          <t>131.4300</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>84675</t>
+          <t>1254602</t>
         </is>
       </c>
     </row>
@@ -596,27 +596,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>13.4100</t>
+          <t>129.3800</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>13.4400</t>
+          <t>130.5700</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>13.2400</t>
+          <t>127.7200</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>13.2600</t>
+          <t>129.3000</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>176549</t>
+          <t>1533527</t>
         </is>
       </c>
     </row>
@@ -628,27 +628,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>13.8300</t>
+          <t>129.7900</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>13.8300</t>
+          <t>130.2700</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13.3032</t>
+          <t>127.1200</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>13.4600</t>
+          <t>128.0100</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>129512</t>
+          <t>1695916</t>
         </is>
       </c>
     </row>
@@ -660,27 +660,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>13.5200</t>
+          <t>127.6300</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>13.7250</t>
+          <t>129.1100</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13.2900</t>
+          <t>126.2100</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>13.5700</t>
+          <t>128.9300</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>96864</t>
+          <t>1282033</t>
         </is>
       </c>
     </row>
@@ -692,27 +692,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>13.1600</t>
+          <t>129.3800</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>13.5700</t>
+          <t>130.2300</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13.0900</t>
+          <t>128.0000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>13.5500</t>
+          <t>128.2500</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>105893</t>
+          <t>1890926</t>
         </is>
       </c>
     </row>
@@ -724,27 +724,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>13.3400</t>
+          <t>128.5100</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>13.3500</t>
+          <t>129.0190</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12.8804</t>
+          <t>127.1550</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>12.9800</t>
+          <t>128.2800</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>145107</t>
+          <t>1772371</t>
         </is>
       </c>
     </row>
@@ -756,27 +756,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>13.0500</t>
+          <t>128.4300</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>13.4200</t>
+          <t>129.3500</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>13.0500</t>
+          <t>127.1800</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>13.2200</t>
+          <t>128.1100</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>147676</t>
+          <t>867312</t>
         </is>
       </c>
     </row>
@@ -788,27 +788,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>13.5300</t>
+          <t>136.0000</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>13.5300</t>
+          <t>136.0500</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13.1000</t>
+          <t>129.7800</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>13.1900</t>
+          <t>129.8700</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>158679</t>
+          <t>1252797</t>
         </is>
       </c>
     </row>
@@ -820,27 +820,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>13.9400</t>
+          <t>135.3000</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>13.9400</t>
+          <t>136.0800</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13.2300</t>
+          <t>133.9900</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>13.5300</t>
+          <t>136.0100</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>104827</t>
+          <t>969054</t>
         </is>
       </c>
     </row>
@@ -852,27 +852,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>13.2400</t>
+          <t>133.0200</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>13.9800</t>
+          <t>134.5400</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13.1550</t>
+          <t>132.6500</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>13.7700</t>
+          <t>133.6700</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>70603</t>
+          <t>1020493</t>
         </is>
       </c>
     </row>
@@ -884,27 +884,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>12.8900</t>
+          <t>133.1100</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>13.3500</t>
+          <t>134.1050</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12.8850</t>
+          <t>132.0440</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>13.3000</t>
+          <t>132.6400</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>130217</t>
+          <t>1188279</t>
         </is>
       </c>
     </row>
@@ -916,27 +916,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>12.6800</t>
+          <t>135.3000</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>13.1800</t>
+          <t>136.0300</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>12.6800</t>
+          <t>133.5600</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>12.8600</t>
+          <t>133.9400</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>113030</t>
+          <t>1250729</t>
         </is>
       </c>
     </row>
@@ -948,27 +948,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>13.0300</t>
+          <t>139.3500</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>13.3900</t>
+          <t>139.7300</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12.7200</t>
+          <t>137.2600</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>12.9600</t>
+          <t>137.6200</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>121009</t>
+          <t>1477480</t>
         </is>
       </c>
     </row>
@@ -980,27 +980,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>12.9800</t>
+          <t>141.8800</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14.0000</t>
+          <t>141.9632</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12.6900</t>
+          <t>138.7600</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>13.2300</t>
+          <t>139.9700</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>112003</t>
+          <t>1740337</t>
         </is>
       </c>
     </row>
@@ -1012,27 +1012,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>13.3500</t>
+          <t>148.8400</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>13.5000</t>
+          <t>149.0000</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13.0700</t>
+          <t>140.0300</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>13.1400</t>
+          <t>142.2900</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>95398</t>
+          <t>4110100</t>
         </is>
       </c>
     </row>
@@ -1044,27 +1044,27 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>13.9700</t>
+          <t>132.8900</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14.0700</t>
+          <t>133.4200</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13.4500</t>
+          <t>131.6600</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>13.4800</t>
+          <t>132.7700</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>69891</t>
+          <t>1809979</t>
         </is>
       </c>
     </row>
@@ -1076,27 +1076,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>13.9200</t>
+          <t>133.2800</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14.1000</t>
+          <t>134.6200</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13.2500</t>
+          <t>132.6700</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>13.9700</t>
+          <t>133.9000</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>155029</t>
+          <t>1291166</t>
         </is>
       </c>
     </row>
@@ -1108,27 +1108,27 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>13.2600</t>
+          <t>132.2600</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>13.9800</t>
+          <t>133.6300</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13.1900</t>
+          <t>131.4300</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>13.9500</t>
+          <t>133.5500</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>129866</t>
+          <t>865778</t>
         </is>
       </c>
     </row>
@@ -1140,27 +1140,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>13.9700</t>
+          <t>132.9100</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>14.1500</t>
+          <t>135.1300</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13.1600</t>
+          <t>131.5900</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>13.2200</t>
+          <t>131.9500</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>76615</t>
+          <t>1162499</t>
         </is>
       </c>
     </row>
@@ -1172,27 +1172,27 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>13.3800</t>
+          <t>131.3700</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14.4643</t>
+          <t>132.7700</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13.3800</t>
+          <t>130.1500</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>13.8800</t>
+          <t>132.5800</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>82533</t>
+          <t>1022142</t>
         </is>
       </c>
     </row>
@@ -1204,27 +1204,27 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>14.1900</t>
+          <t>132.5000</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14.7493</t>
+          <t>132.5000</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13.6700</t>
+          <t>128.0200</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>14.0900</t>
+          <t>128.8800</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>72410</t>
+          <t>894724</t>
         </is>
       </c>
     </row>
@@ -1236,27 +1236,27 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>14.3700</t>
+          <t>134.2000</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>14.6800</t>
+          <t>134.4200</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14.0200</t>
+          <t>132.1400</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>14.2200</t>
+          <t>132.5200</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>72069</t>
+          <t>1257078</t>
         </is>
       </c>
     </row>
@@ -1268,27 +1268,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>13.9600</t>
+          <t>132.2700</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>14.3500</t>
+          <t>133.8400</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>13.7800</t>
+          <t>131.7500</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>14.2000</t>
+          <t>133.6100</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>83472</t>
+          <t>675823</t>
         </is>
       </c>
     </row>
@@ -1300,27 +1300,27 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>13.6200</t>
+          <t>134.6900</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>14.2600</t>
+          <t>135.0000</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>13.6200</t>
+          <t>132.7400</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>14.1100</t>
+          <t>133.7700</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>117008</t>
+          <t>895554</t>
         </is>
       </c>
     </row>
@@ -1332,27 +1332,27 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>13.5600</t>
+          <t>133.4500</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>14.1900</t>
+          <t>135.2600</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>13.3100</t>
+          <t>133.0200</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>13.5200</t>
+          <t>134.5600</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>86025</t>
+          <t>2113206</t>
         </is>
       </c>
     </row>
@@ -1364,27 +1364,27 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>12.3600</t>
+          <t>132.4100</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>13.4700</t>
+          <t>134.6800</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12.3600</t>
+          <t>131.0900</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>13.4300</t>
+          <t>131.2800</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>198124</t>
+          <t>1398687</t>
         </is>
       </c>
     </row>
@@ -1396,27 +1396,27 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>12.1552</t>
+          <t>133.5100</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>12.7400</t>
+          <t>135.2300</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12.0100</t>
+          <t>133.2600</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>12.4300</t>
+          <t>133.4300</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>220546</t>
+          <t>1081837</t>
         </is>
       </c>
     </row>
@@ -1428,27 +1428,27 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>12.5900</t>
+          <t>131.2700</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>12.6300</t>
+          <t>134.5000</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12.0700</t>
+          <t>130.9000</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>12.3700</t>
+          <t>134.1000</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>47409</t>
+          <t>2214917</t>
         </is>
       </c>
     </row>
@@ -1460,27 +1460,27 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>12.9000</t>
+          <t>128.1700</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>13.0000</t>
+          <t>131.8250</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12.6200</t>
+          <t>126.7800</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>12.7100</t>
+          <t>131.1100</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>99639</t>
+          <t>1861392</t>
         </is>
       </c>
     </row>
@@ -1492,27 +1492,27 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>13.0700</t>
+          <t>125.0400</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>13.1000</t>
+          <t>128.3300</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12.8000</t>
+          <t>124.7100</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>13.0000</t>
+          <t>127.7100</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>235697</t>
+          <t>1395945</t>
         </is>
       </c>
     </row>
@@ -1524,27 +1524,27 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>12.7100</t>
+          <t>124.6600</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>13.0400</t>
+          <t>125.6300</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12.7100</t>
+          <t>123.3700</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>12.8200</t>
+          <t>125.1700</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>96802</t>
+          <t>1259957</t>
         </is>
       </c>
     </row>
@@ -1556,27 +1556,27 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>12.7000</t>
+          <t>125.0500</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>13.0100</t>
+          <t>125.4100</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12.4100</t>
+          <t>123.1900</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>12.8500</t>
+          <t>124.2600</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>341666</t>
+          <t>1044007</t>
         </is>
       </c>
     </row>
@@ -1588,27 +1588,27 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>12.8500</t>
+          <t>127.4100</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>12.9300</t>
+          <t>128.5399</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12.5000</t>
+          <t>124.3100</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>12.7700</t>
+          <t>125.0400</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>98198</t>
+          <t>1079466</t>
         </is>
       </c>
     </row>
@@ -1620,27 +1620,27 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>12.7300</t>
+          <t>122.1200</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>13.0100</t>
+          <t>127.3400</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12.6600</t>
+          <t>122.1200</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>12.9600</t>
+          <t>127.1900</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>81865</t>
+          <t>1682559</t>
         </is>
       </c>
     </row>
@@ -1652,27 +1652,27 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>13.0900</t>
+          <t>119.9300</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>13.1000</t>
+          <t>121.2100</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>12.3000</t>
+          <t>119.2500</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>12.7300</t>
+          <t>119.8600</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>64104</t>
+          <t>1316597</t>
         </is>
       </c>
     </row>
@@ -1684,27 +1684,27 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>12.4000</t>
+          <t>116.9900</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>13.0300</t>
+          <t>119.3400</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12.1380</t>
+          <t>116.3700</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>12.8600</t>
+          <t>119.0600</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>56005</t>
+          <t>1296959</t>
         </is>
       </c>
     </row>
@@ -1716,27 +1716,27 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>12.9700</t>
+          <t>118.9500</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>13.2000</t>
+          <t>119.3900</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>12.0900</t>
+          <t>114.4600</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>12.1500</t>
+          <t>115.1100</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>61009</t>
+          <t>1178166</t>
         </is>
       </c>
     </row>
@@ -1748,27 +1748,27 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>13.0000</t>
+          <t>117.7800</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>13.0000</t>
+          <t>118.8800</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12.4500</t>
+          <t>116.0000</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>12.8600</t>
+          <t>118.8300</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>45030</t>
+          <t>969438</t>
         </is>
       </c>
     </row>
@@ -1780,27 +1780,27 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>12.7700</t>
+          <t>117.1000</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>13.0200</t>
+          <t>117.7300</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>12.6000</t>
+          <t>113.0200</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>12.7700</t>
+          <t>115.8800</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>64159</t>
+          <t>1347360</t>
         </is>
       </c>
     </row>
@@ -1812,27 +1812,27 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>12.6900</t>
+          <t>117.4100</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>13.4000</t>
+          <t>119.7000</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12.6550</t>
+          <t>116.8600</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>12.9000</t>
+          <t>118.6500</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>98577</t>
+          <t>1378011</t>
         </is>
       </c>
     </row>
@@ -1844,27 +1844,27 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>13.4000</t>
+          <t>122.4300</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>13.4000</t>
+          <t>123.4100</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12.6600</t>
+          <t>118.7500</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>12.9500</t>
+          <t>119.2400</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>68029</t>
+          <t>1196763</t>
         </is>
       </c>
     </row>
@@ -1876,27 +1876,27 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>13.8000</t>
+          <t>121.6100</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>13.8000</t>
+          <t>123.4600</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13.0500</t>
+          <t>121.0100</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>13.3100</t>
+          <t>123.1200</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>63322</t>
+          <t>1304407</t>
         </is>
       </c>
     </row>
@@ -1908,27 +1908,27 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>13.6100</t>
+          <t>120.9600</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>13.9500</t>
+          <t>123.2100</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13.3000</t>
+          <t>120.9600</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>13.7900</t>
+          <t>122.5100</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>76990</t>
+          <t>1267400</t>
         </is>
       </c>
     </row>
@@ -1940,27 +1940,27 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>13.5400</t>
+          <t>120.9900</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>14.0000</t>
+          <t>123.2200</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13.5400</t>
+          <t>120.6200</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>13.7000</t>
+          <t>123.1500</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>73687</t>
+          <t>1221228</t>
         </is>
       </c>
     </row>
@@ -1972,27 +1972,27 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>13.5000</t>
+          <t>120.8000</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>14.1000</t>
+          <t>122.3400</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13.3050</t>
+          <t>120.5550</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>13.4500</t>
+          <t>121.1800</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>114804</t>
+          <t>1642289</t>
         </is>
       </c>
     </row>
@@ -2004,27 +2004,27 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>12.6400</t>
+          <t>117.7500</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>13.4600</t>
+          <t>120.6750</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12.6400</t>
+          <t>116.4900</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>13.4300</t>
+          <t>120.5600</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>153439</t>
+          <t>1484902</t>
         </is>
       </c>
     </row>
@@ -2036,27 +2036,27 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>12.3600</t>
+          <t>118.7900</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>12.8500</t>
+          <t>119.7600</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12.2600</t>
+          <t>116.7000</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>12.7700</t>
+          <t>119.2100</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>58956</t>
+          <t>1119770</t>
         </is>
       </c>
     </row>
@@ -2068,27 +2068,27 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>12.6200</t>
+          <t>116.0000</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>12.9700</t>
+          <t>119.9500</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12.1800</t>
+          <t>116.0000</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>12.3200</t>
+          <t>118.7700</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>129496</t>
+          <t>1611981</t>
         </is>
       </c>
     </row>
@@ -2100,27 +2100,27 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>11.8300</t>
+          <t>117.1900</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>13.1400</t>
+          <t>118.5400</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>11.7800</t>
+          <t>116.2400</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>12.9800</t>
+          <t>117.9000</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>285677</t>
+          <t>906648</t>
         </is>
       </c>
     </row>
@@ -2132,27 +2132,27 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>12.0800</t>
+          <t>120.4500</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>12.3300</t>
+          <t>121.2400</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>11.7200</t>
+          <t>116.7200</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>11.9200</t>
+          <t>117.0600</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>479875</t>
+          <t>1426079</t>
         </is>
       </c>
     </row>
@@ -2164,27 +2164,27 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>12.2900</t>
+          <t>121.8300</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>12.6150</t>
+          <t>122.2950</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>11.9600</t>
+          <t>119.8500</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>12.1000</t>
+          <t>120.5700</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>165222</t>
+          <t>1805698</t>
         </is>
       </c>
     </row>
@@ -2196,27 +2196,27 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>13.3000</t>
+          <t>119.9500</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>13.5000</t>
+          <t>121.3500</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12.1300</t>
+          <t>118.4460</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>12.1600</t>
+          <t>121.2900</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>1642678</t>
+          <t>3780403</t>
         </is>
       </c>
     </row>
@@ -2228,27 +2228,27 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>12.6500</t>
+          <t>114.6000</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>13.3200</t>
+          <t>118.7500</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12.6500</t>
+          <t>114.2700</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>13.2500</t>
+          <t>118.6000</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>227736</t>
+          <t>1801564</t>
         </is>
       </c>
     </row>
@@ -2260,27 +2260,27 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>12.5000</t>
+          <t>112.6600</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>12.7550</t>
+          <t>115.0800</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12.2500</t>
+          <t>112.5200</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>12.5000</t>
+          <t>113.8000</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>176053</t>
+          <t>2585285</t>
         </is>
       </c>
     </row>
@@ -2292,27 +2292,27 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>14.0100</t>
+          <t>114.4100</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>14.3100</t>
+          <t>115.5700</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12.7300</t>
+          <t>113.7600</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>12.8100</t>
+          <t>113.8800</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>137648</t>
+          <t>1588225</t>
         </is>
       </c>
     </row>
@@ -2324,27 +2324,27 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>12.8400</t>
+          <t>114.7700</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>14.1000</t>
+          <t>116.7300</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12.8400</t>
+          <t>112.6700</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>13.6500</t>
+          <t>112.7100</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>425648</t>
+          <t>2681452</t>
         </is>
       </c>
     </row>
@@ -2356,27 +2356,27 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>13.0200</t>
+          <t>113.8000</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>13.0200</t>
+          <t>115.0800</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12.2000</t>
+          <t>113.3600</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>12.8100</t>
+          <t>114.9600</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>140975</t>
+          <t>1601588</t>
         </is>
       </c>
     </row>
@@ -2388,27 +2388,27 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>13.2000</t>
+          <t>117.2400</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>13.9800</t>
+          <t>117.7700</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13.1250</t>
+          <t>113.7700</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>13.4600</t>
+          <t>116.4700</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>101499</t>
+          <t>1886299</t>
         </is>
       </c>
     </row>
@@ -2420,27 +2420,27 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>12.9700</t>
+          <t>115.9900</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>13.3000</t>
+          <t>116.7000</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>12.2200</t>
+          <t>113.2500</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>13.0800</t>
+          <t>116.0100</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>94705</t>
+          <t>1314047</t>
         </is>
       </c>
     </row>
@@ -2452,27 +2452,27 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>13.3800</t>
+          <t>116.4800</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>13.9600</t>
+          <t>117.7000</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>12.8000</t>
+          <t>115.3800</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>12.8000</t>
+          <t>116.2800</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>134738</t>
+          <t>1405810</t>
         </is>
       </c>
     </row>
@@ -2484,27 +2484,27 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>14.2600</t>
+          <t>121.6300</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14.6900</t>
+          <t>121.9300</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13.7200</t>
+          <t>119.9000</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>14.0600</t>
+          <t>120.5700</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>106110</t>
+          <t>1379592</t>
         </is>
       </c>
     </row>
@@ -2516,27 +2516,27 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>15.8400</t>
+          <t>126.0900</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16.1900</t>
+          <t>126.9200</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>14.6600</t>
+          <t>124.1300</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>14.6700</t>
+          <t>124.1400</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>131240</t>
+          <t>814426</t>
         </is>
       </c>
     </row>
@@ -2548,27 +2548,27 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>15.0200</t>
+          <t>127.8800</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16.4400</t>
+          <t>128.6400</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>15.0200</t>
+          <t>126.4007</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>16.1100</t>
+          <t>126.8400</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>97521</t>
+          <t>1049455</t>
         </is>
       </c>
     </row>
@@ -2580,27 +2580,27 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>15.2700</t>
+          <t>126.5700</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>15.4500</t>
+          <t>131.2000</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>14.4100</t>
+          <t>126.5700</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>15.0800</t>
+          <t>128.9000</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>142435</t>
+          <t>1236306</t>
         </is>
       </c>
     </row>
@@ -2612,27 +2612,27 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>17.0100</t>
+          <t>129.3800</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>17.0100</t>
+          <t>130.0000</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>15.2500</t>
+          <t>126.9700</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>15.3600</t>
+          <t>127.6300</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>155027</t>
+          <t>1310578</t>
         </is>
       </c>
     </row>
@@ -2644,27 +2644,27 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16.6600</t>
+          <t>127.6200</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>17.2700</t>
+          <t>128.7200</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>16.3400</t>
+          <t>126.4150</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>16.5600</t>
+          <t>128.4900</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>85770</t>
+          <t>1722770</t>
         </is>
       </c>
     </row>
@@ -2676,27 +2676,27 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>15.8700</t>
+          <t>122.9600</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16.7400</t>
+          <t>129.1900</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>15.8100</t>
+          <t>122.3000</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>16.7200</t>
+          <t>129.1000</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>98218</t>
+          <t>1444413</t>
         </is>
       </c>
     </row>
@@ -2708,27 +2708,27 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16.1700</t>
+          <t>127.8600</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16.8150</t>
+          <t>128.9800</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>15.6800</t>
+          <t>122.4300</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>15.9500</t>
+          <t>123.0900</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>100096</t>
+          <t>1757620</t>
         </is>
       </c>
     </row>
@@ -2740,27 +2740,27 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>15.2500</t>
+          <t>128.9100</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>16.3300</t>
+          <t>130.0700</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>15.1250</t>
+          <t>126.7200</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>16.1100</t>
+          <t>127.5600</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>101576</t>
+          <t>3403072</t>
         </is>
       </c>
     </row>
@@ -2772,27 +2772,27 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>14.4900</t>
+          <t>124.9200</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>15.3900</t>
+          <t>130.7700</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>13.5200</t>
+          <t>124.4900</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>15.3800</t>
+          <t>130.5500</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>85411</t>
+          <t>2698841</t>
         </is>
       </c>
     </row>
@@ -2804,27 +2804,27 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>13.7800</t>
+          <t>120.7500</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14.4800</t>
+          <t>124.2200</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>13.7800</t>
+          <t>120.7150</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>14.3900</t>
+          <t>123.8500</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>73315</t>
+          <t>1768031</t>
         </is>
       </c>
     </row>
@@ -2836,27 +2836,27 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>14.5300</t>
+          <t>127.2100</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>14.5300</t>
+          <t>127.4600</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>13.5700</t>
+          <t>119.1800</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>13.6900</t>
+          <t>120.3800</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>50840</t>
+          <t>3524637</t>
         </is>
       </c>
     </row>
@@ -2868,27 +2868,27 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>14.4300</t>
+          <t>125.3200</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14.4800</t>
+          <t>126.0000</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>13.7228</t>
+          <t>123.8000</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>13.9100</t>
+          <t>124.4100</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>75527</t>
+          <t>2187684</t>
         </is>
       </c>
     </row>
@@ -2900,27 +2900,27 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>14.9600</t>
+          <t>126.4500</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15.1900</t>
+          <t>126.4700</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14.5600</t>
+          <t>123.7600</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>14.7200</t>
+          <t>125.9800</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>43306</t>
+          <t>2037143</t>
         </is>
       </c>
     </row>
@@ -2932,27 +2932,27 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>14.4900</t>
+          <t>124.0300</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15.5400</t>
+          <t>125.5800</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>13.6500</t>
+          <t>122.4400</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>14.7900</t>
+          <t>125.1300</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>57030</t>
+          <t>2594718</t>
         </is>
       </c>
     </row>
@@ -2964,27 +2964,27 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>13.6400</t>
+          <t>120.3100</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>14.5200</t>
+          <t>123.5800</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>13.5300</t>
+          <t>119.5300</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>14.3500</t>
+          <t>122.4000</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>74004</t>
+          <t>2310072</t>
         </is>
       </c>
     </row>
@@ -2996,27 +2996,27 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>14.5400</t>
+          <t>121.1900</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>14.9950</t>
+          <t>121.9050</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>13.7200</t>
+          <t>120.3100</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>13.8600</t>
+          <t>120.7900</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>107810</t>
+          <t>1335997</t>
         </is>
       </c>
     </row>
@@ -3028,27 +3028,27 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>14.1300</t>
+          <t>122.7000</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>15.1400</t>
+          <t>123.7000</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>13.9700</t>
+          <t>121.4500</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>15.0500</t>
+          <t>123.0800</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>92477</t>
+          <t>2216184</t>
         </is>
       </c>
     </row>
@@ -3060,27 +3060,27 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>14.0400</t>
+          <t>119.6300</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14.7500</t>
+          <t>121.0300</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>13.6500</t>
+          <t>118.8300</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>13.7200</t>
+          <t>120.3000</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>135588</t>
+          <t>2011653</t>
         </is>
       </c>
     </row>
@@ -3092,27 +3092,27 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>12.8700</t>
+          <t>117.3800</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>14.3400</t>
+          <t>120.7150</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>12.8700</t>
+          <t>117.2700</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>14.0200</t>
+          <t>119.3800</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>134672</t>
+          <t>1328411</t>
         </is>
       </c>
     </row>
@@ -3124,27 +3124,27 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>11.0100</t>
+          <t>113.6100</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>12.6600</t>
+          <t>116.2500</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>11.0000</t>
+          <t>112.7800</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>12.6500</t>
+          <t>116.1300</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>201807</t>
+          <t>1338023</t>
         </is>
       </c>
     </row>
@@ -3156,27 +3156,27 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>12.3300</t>
+          <t>115.7000</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>12.9600</t>
+          <t>118.0000</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>11.5100</t>
+          <t>113.8400</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>11.5700</t>
+          <t>113.9900</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>136505</t>
+          <t>1607013</t>
         </is>
       </c>
     </row>
@@ -3188,27 +3188,27 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>13.3900</t>
+          <t>115.4400</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>13.4900</t>
+          <t>117.9400</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>12.1700</t>
+          <t>113.1400</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>12.4000</t>
+          <t>116.6400</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>195240</t>
+          <t>2141753</t>
         </is>
       </c>
     </row>
@@ -3220,27 +3220,27 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>14.1900</t>
+          <t>119.1300</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>14.7800</t>
+          <t>119.1300</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>12.9450</t>
+          <t>112.6400</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>12.9600</t>
+          <t>113.1100</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>137685</t>
+          <t>1861704</t>
         </is>
       </c>
     </row>
@@ -3252,27 +3252,27 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>15.4800</t>
+          <t>120.8800</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>15.4800</t>
+          <t>121.8800</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>14.3450</t>
+          <t>118.0000</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>14.5300</t>
+          <t>121.0800</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>177875</t>
+          <t>1629034</t>
         </is>
       </c>
     </row>
@@ -3284,27 +3284,27 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16.0300</t>
+          <t>124.6200</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>16.5250</t>
+          <t>125.2100</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>15.2750</t>
+          <t>120.8000</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>15.7100</t>
+          <t>122.1500</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>136609</t>
+          <t>2123645</t>
         </is>
       </c>
     </row>
@@ -3316,27 +3316,27 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16.2000</t>
+          <t>121.6900</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>16.5900</t>
+          <t>126.6900</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>15.3100</t>
+          <t>121.4400</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>16.4100</t>
+          <t>126.3000</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>107277</t>
+          <t>2454301</t>
         </is>
       </c>
     </row>
@@ -3348,27 +3348,27 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>15.7100</t>
+          <t>119.7200</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>16.3100</t>
+          <t>123.9800</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>15.2500</t>
+          <t>119.0900</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>16.2500</t>
+          <t>122.4000</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>72081</t>
+          <t>3217838</t>
         </is>
       </c>
     </row>
@@ -3380,27 +3380,27 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>14.6900</t>
+          <t>118.3800</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>15.7700</t>
+          <t>120.3400</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>14.4200</t>
+          <t>116.4900</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>15.7300</t>
+          <t>119.5700</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>179973</t>
+          <t>1756159</t>
         </is>
       </c>
     </row>
@@ -3412,27 +3412,27 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>15.2400</t>
+          <t>120.7100</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>15.6800</t>
+          <t>123.8900</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>14.6000</t>
+          <t>119.0500</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>14.6000</t>
+          <t>119.2700</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>65158</t>
+          <t>2269171</t>
         </is>
       </c>
     </row>
@@ -3444,27 +3444,27 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>15.8100</t>
+          <t>119.5200</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>15.8100</t>
+          <t>121.5600</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>14.6600</t>
+          <t>117.9300</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>15.4300</t>
+          <t>121.0600</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>74828</t>
+          <t>3152172</t>
         </is>
       </c>
     </row>
@@ -3476,27 +3476,27 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>15.5100</t>
+          <t>118.2000</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>15.8100</t>
+          <t>120.8500</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>15.0700</t>
+          <t>117.5300</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>15.4700</t>
+          <t>117.6800</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>64059</t>
+          <t>2007479</t>
         </is>
       </c>
     </row>
@@ -3508,27 +3508,27 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16.0700</t>
+          <t>121.0000</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>16.6500</t>
+          <t>121.2800</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>15.5100</t>
+          <t>117.2400</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>15.5100</t>
+          <t>117.9400</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>105814</t>
+          <t>2928082</t>
         </is>
       </c>
     </row>
@@ -3540,27 +3540,27 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>15.2200</t>
+          <t>119.5300</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>16.3500</t>
+          <t>121.6100</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>15.2200</t>
+          <t>118.2300</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>16.2600</t>
+          <t>121.4500</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>70947</t>
+          <t>2236881</t>
         </is>
       </c>
     </row>
@@ -3572,27 +3572,27 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>15.6600</t>
+          <t>124.7700</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>15.7700</t>
+          <t>125.1000</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>15.1300</t>
+          <t>121.1500</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>15.3500</t>
+          <t>121.3200</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>63336</t>
+          <t>1947222</t>
         </is>
       </c>
     </row>
@@ -3604,27 +3604,27 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16.4800</t>
+          <t>130.3600</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16.4800</t>
+          <t>131.0300</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>15.3100</t>
+          <t>124.8500</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>15.6300</t>
+          <t>125.2900</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>75465</t>
+          <t>2177667</t>
         </is>
       </c>
     </row>
@@ -3636,27 +3636,27 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>16.4400</t>
+          <t>127.7100</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16.6900</t>
+          <t>130.3200</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>15.8000</t>
+          <t>126.8400</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>16.3900</t>
+          <t>129.3700</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>64751</t>
+          <t>2011105</t>
         </is>
       </c>
     </row>

</xml_diff>